<commit_message>
Rearranged tests, projects and npm scripts
</commit_message>
<xml_diff>
--- a/excel-report/PlaywrightDemo_TS.xlsx
+++ b/excel-report/PlaywrightDemo_TS.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24334"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881CD310-519C-4D2A-9A15-78E65856B719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2F887E-1DB2-4D18-9351-F5DD19C7CA65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -23,8 +23,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +30,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -54,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="37">
   <si>
     <t>FullScope (UI)</t>
   </si>
@@ -104,12 +102,6 @@
     <t>Note</t>
   </si>
   <si>
-    <t>This Test should fail</t>
-  </si>
-  <si>
-    <t>This Test should pass</t>
-  </si>
-  <si>
     <t>configuration1</t>
   </si>
   <si>
@@ -117,6 +109,60 @@
   </si>
   <si>
     <t>Configuration</t>
+  </si>
+  <si>
+    <t>Parameterized Test | Create and delete room 994</t>
+  </si>
+  <si>
+    <t>Parameterized Test | Create and delete room 995</t>
+  </si>
+  <si>
+    <t>Teardown Steps</t>
+  </si>
+  <si>
+    <t>Switch Working Context</t>
+  </si>
+  <si>
+    <t>Temporary Data</t>
+  </si>
+  <si>
+    <t>Expected test failure, due to errorListener catching a JS error</t>
+  </si>
+  <si>
+    <t>Expected test failure, due to errorListener catching an Error Status code</t>
+  </si>
+  <si>
+    <t>Expected test failure, due to errorListener catching a Connection Error</t>
+  </si>
+  <si>
+    <t>Setup Steps</t>
+  </si>
+  <si>
+    <t>Login page displayed, when initial tab is instantiated without a storageState</t>
+  </si>
+  <si>
+    <t>Admin Panel displayed, when initial tab is instantiated with a storageState</t>
+  </si>
+  <si>
+    <t>Login page displayed, when the new tab is instantiated in the current context, which was instantiated without storageState</t>
+  </si>
+  <si>
+    <t>Admin Panel page displayed, when the new tab is instantiated in the current context, which was instantiated with storageState</t>
+  </si>
+  <si>
+    <t>Admin Panel page displayed, when the new tab is instantiated in a new context with storageState, while previous context was instantiated without storageState</t>
+  </si>
+  <si>
+    <t>Admin Panel page displayed, when the new tab is instantiated in a new context with storageState, while previous context was instantiated with storageState</t>
+  </si>
+  <si>
+    <t>Switch Working Tab</t>
+  </si>
+  <si>
+    <t>Login page displayed, when the new tab is instantiated in a new context without storageState, while previous context was instantiated without storageState</t>
+  </si>
+  <si>
+    <t>Login page displayed, when the new tab is instantiated in a new context without storageState, while previous context was instantiated with storageState</t>
   </si>
 </sst>
 </file>
@@ -245,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -255,9 +301,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -271,20 +314,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="38">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -302,6 +345,326 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -630,50 +993,50 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="13" t="s">
+      <c r="A3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="13"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="13" t="s">
+      <c r="G3" s="14"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="13"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="13" t="s">
+      <c r="J3" s="14"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="13"/>
-      <c r="N3" s="11"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="10"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
@@ -681,7 +1044,7 @@
         <f>COUNTIFS('FullScope (UI)'!C:C,$A3,'FullScope (UI)'!D:D,"Passed")</f>
         <v>0</v>
       </c>
-      <c r="E4" s="11"/>
+      <c r="E4" s="10"/>
       <c r="F4" s="1" t="s">
         <v>4</v>
       </c>
@@ -689,7 +1052,7 @@
         <f t="array" ref="G4">IFERROR(ROWS(_xlfn._xlws.FILTER('FullScope (UI)'!A:D,('FullScope (UI)'!C:C=$A3)*('FullScope (UI)'!D:D="Passed")*ISNUMBER(MATCH('FullScope (UI)'!A:A,'Regression (UI)'!A:A,0)))),0)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="11"/>
+      <c r="H4" s="10"/>
       <c r="I4" s="1" t="s">
         <v>4</v>
       </c>
@@ -697,7 +1060,7 @@
         <f t="array" ref="J4">IFERROR(ROWS(_xlfn._xlws.FILTER('FullScope (UI)'!A:D,('FullScope (UI)'!C:C=$A3)*('FullScope (UI)'!D:D="Passed")*ISNUMBER(MATCH('FullScope (UI)'!A:A,'Smoke (UI)'!A:A,0)))),0)</f>
         <v>0</v>
       </c>
-      <c r="K4" s="11"/>
+      <c r="K4" s="10"/>
       <c r="L4" s="1" t="s">
         <v>4</v>
       </c>
@@ -705,11 +1068,11 @@
         <f>COUNTIFS('FullScope (API)'!C:C,$A3,'FullScope (API)'!D:D,"Passed")</f>
         <v>0</v>
       </c>
-      <c r="N4" s="11"/>
+      <c r="N4" s="10"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
@@ -717,7 +1080,7 @@
         <f>COUNTIFS('FullScope (UI)'!C:C,$A3,'FullScope (UI)'!D:D,"Failed")</f>
         <v>0</v>
       </c>
-      <c r="E5" s="11"/>
+      <c r="E5" s="10"/>
       <c r="F5" s="1" t="s">
         <v>5</v>
       </c>
@@ -725,7 +1088,7 @@
         <f t="array" ref="G5">IFERROR(ROWS(_xlfn._xlws.FILTER('FullScope (UI)'!A:D,('FullScope (UI)'!C:C=$A3)*('FullScope (UI)'!D:D="Failed")*ISNUMBER(MATCH('FullScope (UI)'!A:A,'Regression (UI)'!A:A,0)))),0)</f>
         <v>0</v>
       </c>
-      <c r="H5" s="11"/>
+      <c r="H5" s="10"/>
       <c r="I5" s="1" t="s">
         <v>5</v>
       </c>
@@ -733,7 +1096,7 @@
         <f t="array" ref="J5">IFERROR(ROWS(_xlfn._xlws.FILTER('FullScope (UI)'!A:D,('FullScope (UI)'!C:C=$A3)*('FullScope (UI)'!D:D="Failed")*ISNUMBER(MATCH('FullScope (UI)'!A:A,'Smoke (UI)'!A:A,0)))),0)</f>
         <v>0</v>
       </c>
-      <c r="K5" s="11"/>
+      <c r="K5" s="10"/>
       <c r="L5" s="1" t="s">
         <v>5</v>
       </c>
@@ -741,141 +1104,141 @@
         <f>COUNTIFS('FullScope (API)'!C:C,$A3,'FullScope (API)'!D:D,"Failed")</f>
         <v>0</v>
       </c>
-      <c r="N5" s="11"/>
+      <c r="N5" s="10"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="2">
         <f>COUNTIFS('FullScope (UI)'!C:C,$A3,'FullScope (UI)'!D:D,"")</f>
-        <v>1</v>
-      </c>
-      <c r="E6" s="11"/>
+        <v>13</v>
+      </c>
+      <c r="E6" s="10"/>
       <c r="F6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G6" s="2" cm="1">
         <f t="array" ref="G6">IFERROR(ROWS(_xlfn._xlws.FILTER('FullScope (UI)'!A:D,('FullScope (UI)'!C:C=$A3)*('FullScope (UI)'!D:D="")*ISNUMBER(MATCH('FullScope (UI)'!A:A,'Regression (UI)'!A:A,0)))),0)</f>
-        <v>1</v>
-      </c>
-      <c r="H6" s="11"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="10"/>
       <c r="I6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="J6" s="2" cm="1">
         <f t="array" ref="J6">IFERROR(ROWS(_xlfn._xlws.FILTER('FullScope (UI)'!A:D,('FullScope (UI)'!C:C=$A3)*('FullScope (UI)'!D:D="")*ISNUMBER(MATCH('FullScope (UI)'!A:A,'Smoke (UI)'!A:A,0)))),0)</f>
-        <v>1</v>
-      </c>
-      <c r="K6" s="11"/>
+        <v>0</v>
+      </c>
+      <c r="K6" s="10"/>
       <c r="L6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="M6" s="2">
         <f>COUNTIFS('FullScope (API)'!C:C,$A3,'FullScope (API)'!D:D,"")</f>
-        <v>1</v>
-      </c>
-      <c r="N6" s="11"/>
+        <v>5</v>
+      </c>
+      <c r="N6" s="10"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="3">
         <f>COUNTIFS('FullScope (UI)'!C:C,$A3,'FullScope (UI)'!A:A,"&lt;&gt;"&amp;"")</f>
-        <v>1</v>
-      </c>
-      <c r="E7" s="11"/>
+        <v>13</v>
+      </c>
+      <c r="E7" s="10"/>
       <c r="F7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G7" s="3">
         <f>COUNTIFS('Regression (UI)'!A:A,"&lt;&gt;"&amp;"",'Regression (UI)'!A:A,"&lt;&gt;"&amp;"ID")</f>
-        <v>1</v>
-      </c>
-      <c r="H7" s="11"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="10"/>
       <c r="I7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="J7" s="3">
         <f>COUNTIFS('Smoke (UI)'!A:A,"&lt;&gt;"&amp;"",'Smoke (UI)'!A:A,"&lt;&gt;"&amp;"ID")</f>
-        <v>1</v>
-      </c>
-      <c r="K7" s="11"/>
+        <v>0</v>
+      </c>
+      <c r="K7" s="10"/>
       <c r="L7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="M7" s="3">
         <f>COUNTIFS('FullScope (API)'!C:C,$A3,'FullScope (API)'!A:A,"&lt;&gt;"&amp;"")</f>
+        <v>5</v>
+      </c>
+      <c r="N7" s="10"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="N7" s="11"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="G11" s="13"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="13" t="s">
+      <c r="G11" s="14"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="J11" s="13"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="13" t="s">
+      <c r="J11" s="14"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="M11" s="13"/>
-      <c r="N11" s="11"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="10"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="1" t="s">
         <v>4</v>
       </c>
@@ -883,7 +1246,7 @@
         <f>COUNTIFS('FullScope (UI)'!C:C,$A11,'FullScope (UI)'!D:D,"Passed")</f>
         <v>0</v>
       </c>
-      <c r="E12" s="11"/>
+      <c r="E12" s="10"/>
       <c r="F12" s="1" t="s">
         <v>4</v>
       </c>
@@ -891,7 +1254,7 @@
         <f t="array" ref="G12">IFERROR(ROWS(_xlfn._xlws.FILTER('FullScope (UI)'!A:D,('FullScope (UI)'!C:C=$A11)*('FullScope (UI)'!D:D="Passed")*ISNUMBER(MATCH('FullScope (UI)'!A:A,'Regression (UI)'!A:A,0)))),0)</f>
         <v>0</v>
       </c>
-      <c r="H12" s="11"/>
+      <c r="H12" s="10"/>
       <c r="I12" s="1" t="s">
         <v>4</v>
       </c>
@@ -899,7 +1262,7 @@
         <f t="array" ref="J12">IFERROR(ROWS(_xlfn._xlws.FILTER('FullScope (UI)'!A:D,('FullScope (UI)'!C:C=$A11)*('FullScope (UI)'!D:D="Passed")*ISNUMBER(MATCH('FullScope (UI)'!A:A,'Smoke (UI)'!A:A,0)))),0)</f>
         <v>0</v>
       </c>
-      <c r="K12" s="11"/>
+      <c r="K12" s="10"/>
       <c r="L12" s="1" t="s">
         <v>4</v>
       </c>
@@ -907,11 +1270,11 @@
         <f>COUNTIFS('FullScope (API)'!C:C,$A11,'FullScope (API)'!D:D,"Passed")</f>
         <v>0</v>
       </c>
-      <c r="N12" s="11"/>
+      <c r="N12" s="10"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="1" t="s">
         <v>5</v>
       </c>
@@ -919,7 +1282,7 @@
         <f>COUNTIFS('FullScope (UI)'!C:C,$A11,'FullScope (UI)'!D:D,"Failed")</f>
         <v>0</v>
       </c>
-      <c r="E13" s="11"/>
+      <c r="E13" s="10"/>
       <c r="F13" s="1" t="s">
         <v>5</v>
       </c>
@@ -927,7 +1290,7 @@
         <f t="array" ref="G13">IFERROR(ROWS(_xlfn._xlws.FILTER('FullScope (UI)'!A:D,('FullScope (UI)'!C:C=$A11)*('FullScope (UI)'!D:D="Failed")*ISNUMBER(MATCH('FullScope (UI)'!A:A,'Regression (UI)'!A:A,0)))),0)</f>
         <v>0</v>
       </c>
-      <c r="H13" s="11"/>
+      <c r="H13" s="10"/>
       <c r="I13" s="1" t="s">
         <v>5</v>
       </c>
@@ -935,7 +1298,7 @@
         <f t="array" ref="J13">IFERROR(ROWS(_xlfn._xlws.FILTER('FullScope (UI)'!A:D,('FullScope (UI)'!C:C=$A11)*('FullScope (UI)'!D:D="Failed")*ISNUMBER(MATCH('FullScope (UI)'!A:A,'Smoke (UI)'!A:A,0)))),0)</f>
         <v>0</v>
       </c>
-      <c r="K13" s="11"/>
+      <c r="K13" s="10"/>
       <c r="L13" s="1" t="s">
         <v>5</v>
       </c>
@@ -943,108 +1306,98 @@
         <f>COUNTIFS('FullScope (API)'!C:C,$A11,'FullScope (API)'!D:D,"Failed")</f>
         <v>0</v>
       </c>
-      <c r="N13" s="11"/>
+      <c r="N13" s="10"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="2">
         <f>COUNTIFS('FullScope (UI)'!C:C,$A11,'FullScope (UI)'!D:D,"")</f>
-        <v>1</v>
-      </c>
-      <c r="E14" s="11"/>
+        <v>13</v>
+      </c>
+      <c r="E14" s="10"/>
       <c r="F14" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G14" s="2" cm="1">
         <f t="array" ref="G14">IFERROR(ROWS(_xlfn._xlws.FILTER('FullScope (UI)'!A:D,('FullScope (UI)'!C:C=$A11)*('FullScope (UI)'!D:D="")*ISNUMBER(MATCH('FullScope (UI)'!A:A,'Regression (UI)'!A:A,0)))),0)</f>
-        <v>1</v>
-      </c>
-      <c r="H14" s="11"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="10"/>
       <c r="I14" s="2" t="s">
         <v>6</v>
       </c>
       <c r="J14" s="2" cm="1">
         <f t="array" ref="J14">IFERROR(ROWS(_xlfn._xlws.FILTER('FullScope (UI)'!A:D,('FullScope (UI)'!C:C=$A11)*('FullScope (UI)'!D:D="")*ISNUMBER(MATCH('FullScope (UI)'!A:A,'Smoke (UI)'!A:A,0)))),0)</f>
-        <v>1</v>
-      </c>
-      <c r="K14" s="11"/>
+        <v>0</v>
+      </c>
+      <c r="K14" s="10"/>
       <c r="L14" s="2" t="s">
         <v>6</v>
       </c>
       <c r="M14" s="2">
         <f>COUNTIFS('FullScope (API)'!C:C,$A11,'FullScope (API)'!D:D,"")</f>
-        <v>1</v>
-      </c>
-      <c r="N14" s="11"/>
+        <v>5</v>
+      </c>
+      <c r="N14" s="10"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
       <c r="C15" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D15" s="3">
         <f>COUNTIFS('FullScope (UI)'!C:C,$A11,'FullScope (UI)'!A:A,"&lt;&gt;"&amp;"")</f>
-        <v>1</v>
-      </c>
-      <c r="E15" s="11"/>
+        <v>13</v>
+      </c>
+      <c r="E15" s="10"/>
       <c r="F15" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G15" s="3">
         <f>COUNTIFS('Regression (UI)'!A:A,"&lt;&gt;"&amp;"",'Regression (UI)'!A:A,"&lt;&gt;"&amp;"ID")</f>
-        <v>1</v>
-      </c>
-      <c r="H15" s="11"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="10"/>
       <c r="I15" s="3" t="s">
         <v>7</v>
       </c>
       <c r="J15" s="3">
         <f>COUNTIFS('Smoke (UI)'!A:A,"&lt;&gt;"&amp;"",'Smoke (UI)'!A:A,"&lt;&gt;"&amp;"ID")</f>
-        <v>1</v>
-      </c>
-      <c r="K15" s="11"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="10"/>
       <c r="L15" s="3" t="s">
         <v>7</v>
       </c>
       <c r="M15" s="3">
         <f>COUNTIFS('FullScope (API)'!C:C,$A11,'FullScope (API)'!A:A,"&lt;&gt;"&amp;"")</f>
-        <v>1</v>
-      </c>
-      <c r="N15" s="11"/>
+        <v>5</v>
+      </c>
+      <c r="N15" s="10"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="11"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A2:N2"/>
-    <mergeCell ref="A3:B7"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="E3:E7"/>
-    <mergeCell ref="H3:H7"/>
-    <mergeCell ref="K3:K7"/>
-    <mergeCell ref="N3:N7"/>
     <mergeCell ref="A16:N16"/>
     <mergeCell ref="A8:N8"/>
     <mergeCell ref="A10:N10"/>
@@ -1057,12 +1410,22 @@
     <mergeCell ref="H11:H15"/>
     <mergeCell ref="K11:K15"/>
     <mergeCell ref="N11:N15"/>
+    <mergeCell ref="A2:N2"/>
+    <mergeCell ref="A3:B7"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="E3:E7"/>
+    <mergeCell ref="H3:H7"/>
+    <mergeCell ref="K3:K7"/>
+    <mergeCell ref="N3:N7"/>
   </mergeCells>
   <conditionalFormatting sqref="A2:N16">
-    <cfRule type="cellIs" dxfId="5" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="26" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="27" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1075,17 +1438,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="147" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" customWidth="1"/>
     <col min="5" max="5" width="5.28515625" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" customWidth="1"/>
@@ -1102,7 +1465,7 @@
         <v>9</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>10</v>
@@ -1125,13 +1488,13 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>18</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -1141,33 +1504,529 @@
       <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
-        <v>1</v>
-      </c>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="5">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>6</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>6</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>7</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>7</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>8</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>9</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>10</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>10</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>11</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>11</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>12</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>12</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>13</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>13</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>14</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>14</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>15</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>15</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>16</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>16</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>17</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>17</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+  <conditionalFormatting sqref="D1:D3 D28:D1048576">
+    <cfRule type="cellIs" dxfId="35" priority="26" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="27" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D5">
+    <cfRule type="cellIs" dxfId="33" priority="23" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="24" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6:D7">
+    <cfRule type="cellIs" dxfId="31" priority="21" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="22" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8:D9">
+    <cfRule type="cellIs" dxfId="29" priority="19" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="20" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10:D11">
+    <cfRule type="cellIs" dxfId="27" priority="17" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="18" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12:D13">
+    <cfRule type="cellIs" dxfId="25" priority="15" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="16" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14:D15">
+    <cfRule type="cellIs" dxfId="23" priority="13" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="14" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16:D17">
+    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="12" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18:D19">
+    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D26:D27">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D20:D23">
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D24:D25">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D27" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Passed,Failed,Blocked"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1180,10 +2039,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1196,11 +2055,6 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
@@ -1211,10 +2065,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1227,11 +2081,6 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
@@ -1242,17 +2091,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" customWidth="1"/>
     <col min="5" max="5" width="5.28515625" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" customWidth="1"/>
@@ -1269,7 +2118,7 @@
         <v>9</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>10</v>
@@ -1291,54 +2140,231 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
-        <v>0</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="A2" s="8">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>0</v>
-      </c>
-      <c r="B3" s="10" t="s">
+      <c r="A3" s="8">
+        <v>0</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>1</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>1</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>2</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>2</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>3</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>3</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>4</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>4</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+  <conditionalFormatting sqref="D1:D9 D12:D1048576">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3" xr:uid="{00000000-0002-0000-0400-000000000000}">
+  <conditionalFormatting sqref="D4:D5">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6:D7">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8:D9">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10:D11">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10:D11">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D11" xr:uid="{7A2EF8FF-829E-42FB-8A36-CBC3931695C4}">
       <formula1>"Passed,Failed,Blocked"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Classified as ECDC NORMAL </oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Updated projects and npm scripts
</commit_message>
<xml_diff>
--- a/excel-report/PlaywrightDemo_TS.xlsx
+++ b/excel-report/PlaywrightDemo_TS.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24334"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2F887E-1DB2-4D18-9351-F5DD19C7CA65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7ABCBBF-CEDB-471C-BB50-89FB53E7F571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -102,12 +102,6 @@
     <t>Note</t>
   </si>
   <si>
-    <t>configuration1</t>
-  </si>
-  <si>
-    <t>configuration2</t>
-  </si>
-  <si>
     <t>Configuration</t>
   </si>
   <si>
@@ -163,6 +157,12 @@
   </si>
   <si>
     <t>Login page displayed, when the new tab is instantiated in a new context without storageState, while previous context was instantiated with storageState</t>
+  </si>
+  <si>
+    <t>chromium-prod</t>
+  </si>
+  <si>
+    <t>firefox-prod</t>
   </si>
 </sst>
 </file>
@@ -987,7 +987,7 @@
   <dimension ref="A2:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A16" sqref="A16:N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,7 +1010,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="12" t="s">
@@ -1212,7 +1212,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="14" t="s">
@@ -1441,14 +1441,14 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="147" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" customWidth="1"/>
     <col min="5" max="5" width="5.28515625" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" customWidth="1"/>
@@ -1465,7 +1465,7 @@
         <v>9</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>10</v>
@@ -1491,10 +1491,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -1508,10 +1508,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -1525,10 +1525,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -1542,10 +1542,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
@@ -1559,10 +1559,10 @@
         <v>7</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -1576,10 +1576,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -1593,10 +1593,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -1610,10 +1610,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
@@ -1627,10 +1627,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -1644,10 +1644,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -1661,10 +1661,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -1678,10 +1678,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -1695,10 +1695,10 @@
         <v>11</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -1712,10 +1712,10 @@
         <v>11</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -1729,10 +1729,10 @@
         <v>12</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
@@ -1746,10 +1746,10 @@
         <v>12</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
@@ -1763,10 +1763,10 @@
         <v>13</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -1780,10 +1780,10 @@
         <v>13</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
@@ -1797,10 +1797,10 @@
         <v>14</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -1814,10 +1814,10 @@
         <v>14</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
@@ -1831,10 +1831,10 @@
         <v>15</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
@@ -1848,10 +1848,10 @@
         <v>15</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
@@ -1865,10 +1865,10 @@
         <v>16</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -1882,10 +1882,10 @@
         <v>16</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
@@ -1899,10 +1899,10 @@
         <v>17</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
@@ -1916,10 +1916,10 @@
         <v>17</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
@@ -2094,14 +2094,14 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="45.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" customWidth="1"/>
     <col min="5" max="5" width="5.28515625" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" customWidth="1"/>
@@ -2118,7 +2118,7 @@
         <v>9</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>10</v>
@@ -2144,10 +2144,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="8"/>
@@ -2161,10 +2161,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="8" t="s">
         <v>17</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="9"/>
@@ -2178,10 +2178,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="8"/>
@@ -2195,10 +2195,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="9"/>
@@ -2212,10 +2212,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="8"/>
@@ -2229,10 +2229,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="9"/>
@@ -2246,10 +2246,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>16</v>
+        <v>20</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="8"/>
@@ -2263,10 +2263,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="9"/>
@@ -2280,10 +2280,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>16</v>
+        <v>21</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="8"/>
@@ -2297,10 +2297,10 @@
         <v>4</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="9"/>

</xml_diff>

<commit_message>
Added faker-js and fakerConfig.spec.ts. Added prettierVerification npm script
</commit_message>
<xml_diff>
--- a/excel-report/PlaywrightDemo_TS.xlsx
+++ b/excel-report/PlaywrightDemo_TS.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24334"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7ABCBBF-CEDB-471C-BB50-89FB53E7F571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DCA0D3A-C1F7-4A43-B917-FCA42E4B2AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="38">
   <si>
     <t>FullScope (UI)</t>
   </si>
@@ -105,12 +105,6 @@
     <t>Configuration</t>
   </si>
   <si>
-    <t>Parameterized Test | Create and delete room 994</t>
-  </si>
-  <si>
-    <t>Parameterized Test | Create and delete room 995</t>
-  </si>
-  <si>
     <t>Teardown Steps</t>
   </si>
   <si>
@@ -163,6 +157,15 @@
   </si>
   <si>
     <t>firefox-prod</t>
+  </si>
+  <si>
+    <t>Parameterized Test | Create and delete Single room</t>
+  </si>
+  <si>
+    <t>Parameterized Test | Create and delete Family room</t>
+  </si>
+  <si>
+    <t>Faker Configuration</t>
   </si>
 </sst>
 </file>
@@ -327,7 +330,47 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="42">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1010,7 +1053,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="12" t="s">
@@ -1138,7 +1181,7 @@
       </c>
       <c r="M6" s="2">
         <f>COUNTIFS('FullScope (API)'!C:C,$A3,'FullScope (API)'!D:D,"")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N6" s="10"/>
     </row>
@@ -1174,7 +1217,7 @@
       </c>
       <c r="M7" s="3">
         <f>COUNTIFS('FullScope (API)'!C:C,$A3,'FullScope (API)'!A:A,"&lt;&gt;"&amp;"")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N7" s="10"/>
     </row>
@@ -1212,7 +1255,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="14" t="s">
@@ -1340,7 +1383,7 @@
       </c>
       <c r="M14" s="2">
         <f>COUNTIFS('FullScope (API)'!C:C,$A11,'FullScope (API)'!D:D,"")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N14" s="10"/>
     </row>
@@ -1376,7 +1419,7 @@
       </c>
       <c r="M15" s="3">
         <f>COUNTIFS('FullScope (API)'!C:C,$A11,'FullScope (API)'!A:A,"&lt;&gt;"&amp;"")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N15" s="10"/>
     </row>
@@ -1422,10 +1465,10 @@
     <mergeCell ref="N3:N7"/>
   </mergeCells>
   <conditionalFormatting sqref="A2:N16">
-    <cfRule type="cellIs" dxfId="37" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="26" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="27" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1440,7 +1483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1491,10 +1534,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -1508,10 +1551,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -1525,10 +1568,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -1542,10 +1585,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
@@ -1559,10 +1602,10 @@
         <v>7</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -1576,10 +1619,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -1593,10 +1636,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -1610,10 +1653,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
@@ -1627,10 +1670,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -1644,10 +1687,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -1661,10 +1704,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -1678,10 +1721,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -1695,10 +1738,10 @@
         <v>11</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -1712,10 +1755,10 @@
         <v>11</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -1729,10 +1772,10 @@
         <v>12</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
@@ -1746,10 +1789,10 @@
         <v>12</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
@@ -1763,10 +1806,10 @@
         <v>13</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -1780,10 +1823,10 @@
         <v>13</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
@@ -1797,10 +1840,10 @@
         <v>14</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -1814,10 +1857,10 @@
         <v>14</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
@@ -1831,10 +1874,10 @@
         <v>15</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
@@ -1848,10 +1891,10 @@
         <v>15</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
@@ -1865,10 +1908,10 @@
         <v>16</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -1882,10 +1925,10 @@
         <v>16</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
@@ -1899,10 +1942,10 @@
         <v>17</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
@@ -1916,10 +1959,10 @@
         <v>17</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
@@ -1930,98 +1973,98 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D3 D28:D1048576">
-    <cfRule type="cellIs" dxfId="35" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="26" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="27" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D5">
-    <cfRule type="cellIs" dxfId="33" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="23" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="24" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:D7">
-    <cfRule type="cellIs" dxfId="31" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="21" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="22" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:D9">
-    <cfRule type="cellIs" dxfId="29" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="19" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="20" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D11">
-    <cfRule type="cellIs" dxfId="27" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="17" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="18" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:D13">
-    <cfRule type="cellIs" dxfId="25" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="15" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="16" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14:D15">
-    <cfRule type="cellIs" dxfId="23" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="13" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="14" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:D17">
-    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="11" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="12" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18:D19">
-    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="9" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="10" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26:D27">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20:D23">
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24:D25">
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2091,10 +2134,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2144,10 +2187,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="8"/>
@@ -2161,10 +2204,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="9"/>
@@ -2178,10 +2221,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="8"/>
@@ -2195,10 +2238,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="9"/>
@@ -2212,10 +2255,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="8"/>
@@ -2229,10 +2272,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="9"/>
@@ -2246,10 +2289,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="8"/>
@@ -2263,10 +2306,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="9"/>
@@ -2280,10 +2323,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="8"/>
@@ -2297,10 +2340,10 @@
         <v>4</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="9"/>
@@ -2309,16 +2352,66 @@
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
     </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>18</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>18</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D9 D12:D1048576">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+  <conditionalFormatting sqref="D1:D9 D14:D1048576">
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="17" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D5">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6:D7">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8:D9">
     <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
@@ -2326,7 +2419,7 @@
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6:D7">
+  <conditionalFormatting sqref="D10:D11">
     <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
@@ -2334,7 +2427,7 @@
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D9">
+  <conditionalFormatting sqref="D10:D11">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
@@ -2342,7 +2435,7 @@
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D10:D11">
+  <conditionalFormatting sqref="D12:D13">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
@@ -2350,7 +2443,7 @@
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D10:D11">
+  <conditionalFormatting sqref="D12:D13">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
@@ -2359,7 +2452,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D11" xr:uid="{7A2EF8FF-829E-42FB-8A36-CBC3931695C4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D13" xr:uid="{7A2EF8FF-829E-42FB-8A36-CBC3931695C4}">
       <formula1>"Passed,Failed,Blocked"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Fixed fakerConfig. Updated all Test IDs
</commit_message>
<xml_diff>
--- a/excel-report/PlaywrightDemo_TS.xlsx
+++ b/excel-report/PlaywrightDemo_TS.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24334"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DCA0D3A-C1F7-4A43-B917-FCA42E4B2AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CCC038A-3526-45EA-A987-9922B8A9CF77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -317,13 +317,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1056,25 +1056,25 @@
         <v>33</v>
       </c>
       <c r="B3" s="11"/>
-      <c r="C3" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="13"/>
+      <c r="C3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="14"/>
       <c r="E3" s="10"/>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="14"/>
+      <c r="G3" s="12"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="14"/>
+      <c r="J3" s="12"/>
       <c r="K3" s="10"/>
-      <c r="L3" s="14" t="s">
+      <c r="L3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="14"/>
+      <c r="M3" s="12"/>
       <c r="N3" s="10"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1258,25 +1258,25 @@
         <v>34</v>
       </c>
       <c r="B11" s="11"/>
-      <c r="C11" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="14"/>
+      <c r="C11" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="12"/>
       <c r="E11" s="10"/>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="G11" s="14"/>
+      <c r="G11" s="12"/>
       <c r="H11" s="10"/>
-      <c r="I11" s="14" t="s">
+      <c r="I11" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="J11" s="14"/>
+      <c r="J11" s="12"/>
       <c r="K11" s="10"/>
-      <c r="L11" s="14" t="s">
+      <c r="L11" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="M11" s="14"/>
+      <c r="M11" s="12"/>
       <c r="N11" s="10"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -1441,6 +1441,16 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A2:N2"/>
+    <mergeCell ref="A3:B7"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="E3:E7"/>
+    <mergeCell ref="H3:H7"/>
+    <mergeCell ref="K3:K7"/>
+    <mergeCell ref="N3:N7"/>
     <mergeCell ref="A16:N16"/>
     <mergeCell ref="A8:N8"/>
     <mergeCell ref="A10:N10"/>
@@ -1453,16 +1463,6 @@
     <mergeCell ref="H11:H15"/>
     <mergeCell ref="K11:K15"/>
     <mergeCell ref="N11:N15"/>
-    <mergeCell ref="A2:N2"/>
-    <mergeCell ref="A3:B7"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="E3:E7"/>
-    <mergeCell ref="H3:H7"/>
-    <mergeCell ref="K3:K7"/>
-    <mergeCell ref="N3:N7"/>
   </mergeCells>
   <conditionalFormatting sqref="A2:N16">
     <cfRule type="cellIs" dxfId="41" priority="26" operator="equal">
@@ -1483,8 +1483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1531,7 +1531,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>20</v>
@@ -1548,7 +1548,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>20</v>
@@ -1565,7 +1565,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>21</v>
@@ -1582,7 +1582,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>21</v>
@@ -1599,7 +1599,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>22</v>
@@ -1616,7 +1616,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>22</v>
@@ -1633,7 +1633,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>23</v>
@@ -1650,7 +1650,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>23</v>
@@ -1667,7 +1667,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>24</v>
@@ -1684,7 +1684,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>24</v>
@@ -1701,7 +1701,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>25</v>
@@ -1718,7 +1718,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>25</v>
@@ -1735,7 +1735,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>26</v>
@@ -1752,7 +1752,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>26</v>
@@ -1769,7 +1769,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>31</v>
@@ -1786,7 +1786,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>31</v>
@@ -1803,7 +1803,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>28</v>
@@ -1820,7 +1820,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>28</v>
@@ -1837,7 +1837,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>27</v>
@@ -1854,7 +1854,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>27</v>
@@ -1871,7 +1871,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>32</v>
@@ -1888,7 +1888,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>32</v>
@@ -1905,7 +1905,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>29</v>
@@ -1922,7 +1922,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>29</v>
@@ -1939,7 +1939,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>30</v>
@@ -1956,7 +1956,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>30</v>
@@ -2111,7 +2111,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2137,7 +2137,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2184,7 +2184,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>35</v>
@@ -2201,7 +2201,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>35</v>
@@ -2218,7 +2218,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>36</v>
@@ -2235,7 +2235,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>36</v>
@@ -2252,7 +2252,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>17</v>
@@ -2269,7 +2269,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>17</v>
@@ -2286,7 +2286,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>18</v>
@@ -2303,7 +2303,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>18</v>
@@ -2320,7 +2320,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>19</v>
@@ -2337,7 +2337,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>19</v>
@@ -2354,7 +2354,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>37</v>
@@ -2371,7 +2371,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Fixed openNewTabInCurrentContext and openNewTabInNewContext to update the pageType for current page
</commit_message>
<xml_diff>
--- a/excel-report/PlaywrightDemo_TS.xlsx
+++ b/excel-report/PlaywrightDemo_TS.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24334"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CCC038A-3526-45EA-A987-9922B8A9CF77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F8B665-E2F7-45FF-8047-6573BA00A88D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,9 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -52,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="39">
   <si>
     <t>FullScope (UI)</t>
   </si>
@@ -166,6 +169,9 @@
   </si>
   <si>
     <t>Faker Configuration</t>
+  </si>
+  <si>
+    <t>Verify Tab Types</t>
   </si>
 </sst>
 </file>
@@ -317,20 +323,40 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="44">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1056,25 +1082,25 @@
         <v>33</v>
       </c>
       <c r="B3" s="11"/>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="14"/>
+      <c r="D3" s="13"/>
       <c r="E3" s="10"/>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="12"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="12"/>
+      <c r="J3" s="14"/>
       <c r="K3" s="10"/>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="12"/>
+      <c r="M3" s="14"/>
       <c r="N3" s="10"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1157,7 +1183,7 @@
       </c>
       <c r="D6" s="2">
         <f>COUNTIFS('FullScope (UI)'!C:C,$A3,'FullScope (UI)'!D:D,"")</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="2" t="s">
@@ -1193,7 +1219,7 @@
       </c>
       <c r="D7" s="3">
         <f>COUNTIFS('FullScope (UI)'!C:C,$A3,'FullScope (UI)'!A:A,"&lt;&gt;"&amp;"")</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="3" t="s">
@@ -1258,25 +1284,25 @@
         <v>34</v>
       </c>
       <c r="B11" s="11"/>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="12"/>
+      <c r="D11" s="14"/>
       <c r="E11" s="10"/>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="G11" s="12"/>
+      <c r="G11" s="14"/>
       <c r="H11" s="10"/>
-      <c r="I11" s="12" t="s">
+      <c r="I11" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="J11" s="12"/>
+      <c r="J11" s="14"/>
       <c r="K11" s="10"/>
-      <c r="L11" s="12" t="s">
+      <c r="L11" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="M11" s="12"/>
+      <c r="M11" s="14"/>
       <c r="N11" s="10"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -1359,7 +1385,7 @@
       </c>
       <c r="D14" s="2">
         <f>COUNTIFS('FullScope (UI)'!C:C,$A11,'FullScope (UI)'!D:D,"")</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="2" t="s">
@@ -1395,7 +1421,7 @@
       </c>
       <c r="D15" s="3">
         <f>COUNTIFS('FullScope (UI)'!C:C,$A11,'FullScope (UI)'!A:A,"&lt;&gt;"&amp;"")</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="3" t="s">
@@ -1441,16 +1467,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A2:N2"/>
-    <mergeCell ref="A3:B7"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="E3:E7"/>
-    <mergeCell ref="H3:H7"/>
-    <mergeCell ref="K3:K7"/>
-    <mergeCell ref="N3:N7"/>
     <mergeCell ref="A16:N16"/>
     <mergeCell ref="A8:N8"/>
     <mergeCell ref="A10:N10"/>
@@ -1463,12 +1479,22 @@
     <mergeCell ref="H11:H15"/>
     <mergeCell ref="K11:K15"/>
     <mergeCell ref="N11:N15"/>
+    <mergeCell ref="A2:N2"/>
+    <mergeCell ref="A3:B7"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="E3:E7"/>
+    <mergeCell ref="H3:H7"/>
+    <mergeCell ref="K3:K7"/>
+    <mergeCell ref="N3:N7"/>
   </mergeCells>
   <conditionalFormatting sqref="A2:N16">
-    <cfRule type="cellIs" dxfId="41" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="26" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="27" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1481,10 +1507,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1971,16 +1997,58 @@
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
     </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>20</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>20</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D3 D28:D1048576">
-    <cfRule type="cellIs" dxfId="39" priority="26" operator="equal">
+  <conditionalFormatting sqref="D1:D3 D30:D1048576">
+    <cfRule type="cellIs" dxfId="41" priority="28" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="29" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D5">
+    <cfRule type="cellIs" dxfId="39" priority="25" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="26" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6:D7">
     <cfRule type="cellIs" dxfId="37" priority="23" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
@@ -1988,7 +2056,7 @@
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6:D7">
+  <conditionalFormatting sqref="D8:D9">
     <cfRule type="cellIs" dxfId="35" priority="21" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
@@ -1996,7 +2064,7 @@
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D9">
+  <conditionalFormatting sqref="D10:D11">
     <cfRule type="cellIs" dxfId="33" priority="19" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
@@ -2004,7 +2072,7 @@
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D10:D11">
+  <conditionalFormatting sqref="D12:D13">
     <cfRule type="cellIs" dxfId="31" priority="17" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
@@ -2012,7 +2080,7 @@
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D12:D13">
+  <conditionalFormatting sqref="D14:D15">
     <cfRule type="cellIs" dxfId="29" priority="15" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
@@ -2020,7 +2088,7 @@
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14:D15">
+  <conditionalFormatting sqref="D16:D17">
     <cfRule type="cellIs" dxfId="27" priority="13" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
@@ -2028,7 +2096,7 @@
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D16:D17">
+  <conditionalFormatting sqref="D18:D19">
     <cfRule type="cellIs" dxfId="25" priority="11" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
@@ -2036,23 +2104,23 @@
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D18:D19">
-    <cfRule type="cellIs" dxfId="23" priority="9" operator="equal">
+  <conditionalFormatting sqref="D26:D27">
+    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="10" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D26:D27">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20:D23">
+    <cfRule type="cellIs" dxfId="21" priority="7" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="8" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D24:D25">
     <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
@@ -2060,16 +2128,16 @@
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D24:D25">
-    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
+  <conditionalFormatting sqref="D28:D29">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D27" xr:uid="{00000000-0002-0000-0100-000000000000}">
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D29" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Passed,Failed,Blocked"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2388,66 +2456,66 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D9 D14:D1048576">
-    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D5">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:D7">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:D9">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D11">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D11">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:D13">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:D13">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>